<commit_message>
yksi virhe korjattu pääohjelmasta
</commit_message>
<xml_diff>
--- a/Parse_log/Parse_log/bin/Debug/net6.0/subdir/test.xlsx
+++ b/Parse_log/Parse_log/bin/Debug/net6.0/subdir/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\genretech\loginPuhdistus\Parse_log\Parse_log\bin\Debug\net6.0\subdir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E367566E-C14B-4B12-A3F8-0103DDFE8782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D6E8F6B-F560-4D68-A3F5-41162BA5601E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-240" windowWidth="20730" windowHeight="11160" xr2:uid="{183D516B-4C47-42FF-A6EA-F873C14F7660}"/>
+    <workbookView xWindow="25395" yWindow="-2235" windowWidth="20400" windowHeight="10920" xr2:uid="{6D69CDA1-1919-4F7D-B954-6CD6DEB2DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50A443D-D83A-49FE-AD0D-46D4D10C4512}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24667DA-8527-45A9-B6AF-E7D5E2267A3C}">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -876,7 +876,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N7" xr:uid="{D50A443D-D83A-49FE-AD0D-46D4D10C4512}"/>
+  <autoFilter ref="A1:N7" xr:uid="{A24667DA-8527-45A9-B6AF-E7D5E2267A3C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Projekti valmis. Timestampin eteen lisätty @-symboli, joka estää exceliä autoformatoimasta timestamppia. Kontrastit katsottu työkalulla läpi, niin että jokainen testi oli ok. Optimointia ei pahemmin löytynyt, ilman syvällisempää tutkimista.
</commit_message>
<xml_diff>
--- a/Parse_log/Parse_log/bin/Debug/net6.0/subdir/test.xlsx
+++ b/Parse_log/Parse_log/bin/Debug/net6.0/subdir/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\genretech\loginPuhdistus\Parse_log\Parse_log\bin\Debug\net6.0\subdir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D6E8F6B-F560-4D68-A3F5-41162BA5601E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BB6E5B5-437F-4CE4-AD49-BFA869A9099E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25395" yWindow="-2235" windowWidth="20400" windowHeight="10920" xr2:uid="{6D69CDA1-1919-4F7D-B954-6CD6DEB2DE47}"/>
+    <workbookView xWindow="25395" yWindow="-2235" windowWidth="20400" windowHeight="10920" xr2:uid="{97A175C0-3938-414F-A867-A66256C5D74F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24667DA-8527-45A9-B6AF-E7D5E2267A3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DB569B-778D-43F4-BECC-1FEF9C104FC4}">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -876,7 +876,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N7" xr:uid="{A24667DA-8527-45A9-B6AF-E7D5E2267A3C}"/>
+  <autoFilter ref="A1:N7" xr:uid="{F4DB569B-778D-43F4-BECC-1FEF9C104FC4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>